<commit_message>
Update butterfly brood table.xlsx
</commit_message>
<xml_diff>
--- a/data/butterfly brood table.xlsx
+++ b/data/butterfly brood table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Butterfly_Project_MBiol\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4F7890-F071-41B8-B007-E354971FA646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD9B26C-B06B-4C3B-9231-000967B9BFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="8700" windowWidth="29040" windowHeight="15840" xr2:uid="{56B928B0-32FD-6245-95ED-D0D0B3954490}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{56B928B0-32FD-6245-95ED-D0D0B3954490}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="137">
   <si>
     <t>Taxonomic species</t>
   </si>
@@ -377,9 +377,6 @@
     <t>August</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>odd one, longdev period</t>
   </si>
   <si>
@@ -419,24 +416,6 @@
     <t>odd as went extinct</t>
   </si>
   <si>
-    <t>Brood1_Temp1</t>
-  </si>
-  <si>
-    <t>Brood1_Temp2</t>
-  </si>
-  <si>
-    <t>Brood2_Temp1</t>
-  </si>
-  <si>
-    <t>Brood2_Temp2</t>
-  </si>
-  <si>
-    <t>Temp 1 = Season in which brood develops</t>
-  </si>
-  <si>
-    <t>Temp2 = Season in which eggs were laid in</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -447,6 +426,27 @@
   </si>
   <si>
     <t>SUMMER</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>FirstMonthOf2ndBrood</t>
+  </si>
+  <si>
+    <t>Brood1_TempDEVELOP </t>
+  </si>
+  <si>
+    <t>Brood2_TempDEVELOP </t>
+  </si>
+  <si>
+    <t>Brood1_TempLAY</t>
+  </si>
+  <si>
+    <t>Brood2_TempLAY</t>
+  </si>
+  <si>
+    <t>NOTES</t>
   </si>
 </sst>
 </file>
@@ -511,26 +511,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FA22C5D-176D-AA49-8395-1796A486F3FC}" name="Table1" displayName="Table1" ref="A1:L209" totalsRowShown="0">
-  <autoFilter ref="A1:L209" xr:uid="{2FA22C5D-176D-AA49-8395-1796A486F3FC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G103">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FA22C5D-176D-AA49-8395-1796A486F3FC}" name="Table1" displayName="Table1" ref="A1:M209" totalsRowShown="0">
+  <autoFilter ref="A1:M209" xr:uid="{2FA22C5D-176D-AA49-8395-1796A486F3FC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H103">
     <sortCondition descending="1" ref="B2:B103"/>
     <sortCondition descending="1" ref="C2:C103"/>
     <sortCondition ref="A2:A103"/>
   </sortState>
-  <tableColumns count="12">
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{3601996E-2C3E-8142-BC83-5F7335E5E718}" name="Taxonomic species"/>
     <tableColumn id="2" xr3:uid="{BBF797C0-B981-2543-83B2-6F548250D9DF}" name="Include"/>
     <tableColumn id="3" xr3:uid="{0CE60A84-0487-5147-94CC-D0076335687C}" name="Univoltine"/>
     <tableColumn id="4" xr3:uid="{501BB500-DD58-A947-900A-F0A3A37C1B60}" name="Month"/>
+    <tableColumn id="13" xr3:uid="{F7D7BE5B-CE4A-4701-A087-7F9F6E9554B0}" name="FirstMonthOf2ndBrood"/>
     <tableColumn id="5" xr3:uid="{4CA5762C-2EE9-3A42-BD8F-D88788D343F9}" name="Brood 1 dev period"/>
     <tableColumn id="6" xr3:uid="{ED2FC863-549D-CA48-A9C7-55855A1A2F7F}" name="Brood 2 dev period"/>
-    <tableColumn id="7" xr3:uid="{6CD8955B-6E7C-564F-B9AF-96E2F29B1E81}" name="Column1"/>
-    <tableColumn id="8" xr3:uid="{2E6D0983-E3E0-4E2B-8244-A8CDF3940F5E}" name="Brood1_Temp1"/>
-    <tableColumn id="9" xr3:uid="{E403E03C-B72B-46C6-B674-8937E304FDB6}" name="Brood1_Temp2"/>
-    <tableColumn id="10" xr3:uid="{BCBBC58F-E92E-400D-8FFB-43A1E00093CC}" name="Brood2_Temp1"/>
-    <tableColumn id="11" xr3:uid="{49621CBD-7AC2-4720-9EC5-C0CAFFE844A8}" name="Brood2_Temp2"/>
-    <tableColumn id="12" xr3:uid="{2E8ED91B-5795-40A3-9FC4-47B4FFAA76AB}" name="Temp 1 = Season in which brood develops"/>
+    <tableColumn id="7" xr3:uid="{6CD8955B-6E7C-564F-B9AF-96E2F29B1E81}" name="NOTES"/>
+    <tableColumn id="8" xr3:uid="{2E6D0983-E3E0-4E2B-8244-A8CDF3940F5E}" name="Brood1_TempDEVELOP "/>
+    <tableColumn id="9" xr3:uid="{E403E03C-B72B-46C6-B674-8937E304FDB6}" name="Brood1_TempLAY"/>
+    <tableColumn id="10" xr3:uid="{BCBBC58F-E92E-400D-8FFB-43A1E00093CC}" name="Brood2_TempDEVELOP "/>
+    <tableColumn id="11" xr3:uid="{49621CBD-7AC2-4720-9EC5-C0CAFFE844A8}" name="Brood2_TempLAY"/>
+    <tableColumn id="12" xr3:uid="{2E8ED91B-5795-40A3-9FC4-47B4FFAA76AB}" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -853,23 +854,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A24936-E824-B74E-933F-86465AE8095B}">
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44:K57"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="13.375" customWidth="1"/>
-    <col min="8" max="8" width="18.375" customWidth="1"/>
-    <col min="9" max="9" width="18.625" customWidth="1"/>
-    <col min="11" max="11" width="19.75" customWidth="1"/>
+    <col min="2" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="27.25" customWidth="1"/>
+    <col min="6" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="13.375" customWidth="1"/>
+    <col min="9" max="9" width="18.375" customWidth="1"/>
+    <col min="10" max="10" width="18.625" customWidth="1"/>
+    <col min="12" max="12" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,32 +885,35 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>113</v>
-      </c>
       <c r="H1" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="I1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="J1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="K1" t="s">
+        <v>133</v>
+      </c>
+      <c r="L1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M1" t="s">
         <v>130</v>
       </c>
-      <c r="L1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -921,25 +927,25 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" t="s">
         <v>110</v>
       </c>
-      <c r="H2" t="s">
-        <v>134</v>
-      </c>
       <c r="I2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="L2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -953,22 +959,25 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" t="s">
         <v>108</v>
       </c>
-      <c r="H3" t="s">
-        <v>134</v>
-      </c>
       <c r="I3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -982,22 +991,25 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" t="s">
         <v>108</v>
       </c>
-      <c r="H4" t="s">
-        <v>134</v>
-      </c>
       <c r="I4" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1011,25 +1023,28 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" t="s">
         <v>108</v>
       </c>
-      <c r="G5" t="s">
-        <v>117</v>
-      </c>
       <c r="H5" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="I5" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -1043,22 +1058,25 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" t="s">
         <v>107</v>
       </c>
-      <c r="H6" t="s">
-        <v>134</v>
-      </c>
       <c r="I6" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1072,22 +1090,25 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" t="s">
         <v>111</v>
       </c>
-      <c r="H7" t="s">
-        <v>134</v>
-      </c>
       <c r="I7" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J7" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1101,22 +1122,25 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" t="s">
         <v>112</v>
       </c>
-      <c r="H8" t="s">
-        <v>134</v>
-      </c>
       <c r="I8" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J8" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>97</v>
       </c>
@@ -1130,22 +1154,25 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F9" t="s">
         <v>108</v>
       </c>
-      <c r="H9" t="s">
-        <v>134</v>
-      </c>
       <c r="I9" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J9" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1159,22 +1186,25 @@
         <v>6</v>
       </c>
       <c r="E10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" t="s">
         <v>111</v>
       </c>
-      <c r="H10" t="s">
-        <v>134</v>
-      </c>
       <c r="I10" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1188,22 +1218,25 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F11" t="s">
         <v>110</v>
       </c>
-      <c r="H11" t="s">
-        <v>134</v>
-      </c>
       <c r="I11" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J11" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1217,22 +1250,25 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" t="s">
         <v>111</v>
       </c>
-      <c r="H12" t="s">
-        <v>134</v>
-      </c>
       <c r="I12" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J12" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -1246,22 +1282,25 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13" t="s">
         <v>111</v>
       </c>
-      <c r="H13" t="s">
-        <v>134</v>
-      </c>
       <c r="I13" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J13" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1275,22 +1314,25 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" t="s">
         <v>108</v>
       </c>
-      <c r="H14" t="s">
-        <v>134</v>
-      </c>
       <c r="I14" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J14" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1304,22 +1346,25 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15" t="s">
         <v>111</v>
       </c>
-      <c r="H15" t="s">
-        <v>134</v>
-      </c>
       <c r="I15" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J15" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1333,22 +1378,25 @@
         <v>8</v>
       </c>
       <c r="E16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" t="s">
         <v>112</v>
       </c>
-      <c r="H16" t="s">
-        <v>134</v>
-      </c>
       <c r="I16" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J16" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1362,22 +1410,25 @@
         <v>6</v>
       </c>
       <c r="E17" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17" t="s">
         <v>111</v>
       </c>
-      <c r="H17" t="s">
-        <v>134</v>
-      </c>
       <c r="I17" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J17" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K17" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1391,22 +1442,25 @@
         <v>6</v>
       </c>
       <c r="E18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" t="s">
         <v>111</v>
       </c>
-      <c r="H18" t="s">
-        <v>134</v>
-      </c>
       <c r="I18" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J18" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K18" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1420,22 +1474,25 @@
         <v>6</v>
       </c>
       <c r="E19" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19" t="s">
         <v>111</v>
       </c>
-      <c r="H19" t="s">
-        <v>134</v>
-      </c>
       <c r="I19" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J19" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -1449,22 +1506,25 @@
         <v>5</v>
       </c>
       <c r="E20" t="s">
+        <v>126</v>
+      </c>
+      <c r="F20" t="s">
         <v>110</v>
       </c>
-      <c r="H20" t="s">
-        <v>134</v>
-      </c>
       <c r="I20" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J20" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1478,22 +1538,25 @@
         <v>6</v>
       </c>
       <c r="E21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F21" t="s">
         <v>111</v>
       </c>
-      <c r="H21" t="s">
-        <v>134</v>
-      </c>
       <c r="I21" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J21" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K21" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -1507,25 +1570,28 @@
         <v>5</v>
       </c>
       <c r="E22" t="s">
+        <v>126</v>
+      </c>
+      <c r="F22" t="s">
         <v>110</v>
       </c>
-      <c r="G22" t="s">
-        <v>121</v>
-      </c>
       <c r="H22" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="I22" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J22" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1539,22 +1605,25 @@
         <v>6</v>
       </c>
       <c r="E23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23" t="s">
         <v>111</v>
       </c>
-      <c r="H23" t="s">
-        <v>134</v>
-      </c>
       <c r="I23" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J23" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K23" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1568,22 +1637,25 @@
         <v>5</v>
       </c>
       <c r="E24" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" t="s">
         <v>110</v>
       </c>
-      <c r="H24" t="s">
-        <v>134</v>
-      </c>
       <c r="I24" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J24" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K24" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -1597,22 +1669,25 @@
         <v>8</v>
       </c>
       <c r="E25" t="s">
+        <v>126</v>
+      </c>
+      <c r="F25" t="s">
         <v>112</v>
       </c>
-      <c r="H25" t="s">
-        <v>134</v>
-      </c>
       <c r="I25" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J25" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1626,22 +1701,25 @@
         <v>7</v>
       </c>
       <c r="E26" t="s">
+        <v>126</v>
+      </c>
+      <c r="F26" t="s">
         <v>108</v>
       </c>
-      <c r="H26" t="s">
-        <v>134</v>
-      </c>
       <c r="I26" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J26" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K26" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>96</v>
       </c>
@@ -1655,25 +1733,28 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27" t="s">
         <v>108</v>
       </c>
-      <c r="G27" t="s">
-        <v>126</v>
-      </c>
       <c r="H27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="I27" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J27" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K27" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -1687,22 +1768,25 @@
         <v>8</v>
       </c>
       <c r="E28" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" t="s">
         <v>112</v>
       </c>
-      <c r="H28" t="s">
-        <v>134</v>
-      </c>
       <c r="I28" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J28" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K28" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1716,22 +1800,25 @@
         <v>6</v>
       </c>
       <c r="E29" t="s">
+        <v>126</v>
+      </c>
+      <c r="F29" t="s">
         <v>111</v>
       </c>
-      <c r="H29" t="s">
-        <v>134</v>
-      </c>
       <c r="I29" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J29" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K29" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -1745,22 +1832,25 @@
         <v>7</v>
       </c>
       <c r="E30" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" t="s">
         <v>108</v>
       </c>
-      <c r="H30" t="s">
-        <v>134</v>
-      </c>
       <c r="I30" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J30" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K30" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1774,22 +1864,25 @@
         <v>5</v>
       </c>
       <c r="E31" t="s">
+        <v>126</v>
+      </c>
+      <c r="F31" t="s">
         <v>110</v>
       </c>
-      <c r="H31" t="s">
-        <v>134</v>
-      </c>
       <c r="I31" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J31" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K31" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -1803,22 +1896,25 @@
         <v>7</v>
       </c>
       <c r="E32" t="s">
+        <v>126</v>
+      </c>
+      <c r="F32" t="s">
         <v>108</v>
       </c>
-      <c r="H32" t="s">
-        <v>134</v>
-      </c>
       <c r="I32" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J32" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K32" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1832,22 +1928,25 @@
         <v>7</v>
       </c>
       <c r="E33" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" t="s">
         <v>108</v>
       </c>
-      <c r="H33" t="s">
-        <v>134</v>
-      </c>
       <c r="I33" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J33" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1861,22 +1960,25 @@
         <v>7</v>
       </c>
       <c r="E34" t="s">
+        <v>126</v>
+      </c>
+      <c r="F34" t="s">
         <v>108</v>
       </c>
-      <c r="H34" t="s">
-        <v>134</v>
-      </c>
       <c r="I34" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J34" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K34" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -1890,25 +1992,28 @@
         <v>4</v>
       </c>
       <c r="E35" t="s">
+        <v>126</v>
+      </c>
+      <c r="F35" t="s">
         <v>107</v>
       </c>
-      <c r="G35" t="s">
-        <v>121</v>
-      </c>
       <c r="H35" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="I35" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J35" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K35" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>84</v>
       </c>
@@ -1922,22 +2027,25 @@
         <v>6</v>
       </c>
       <c r="E36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F36" t="s">
         <v>111</v>
       </c>
-      <c r="H36" t="s">
-        <v>134</v>
-      </c>
       <c r="I36" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J36" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K36" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -1951,22 +2059,25 @@
         <v>106</v>
       </c>
       <c r="E37" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37" t="s">
         <v>112</v>
       </c>
-      <c r="H37" t="s">
-        <v>134</v>
-      </c>
       <c r="I37" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J37" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K37" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -1980,25 +2091,28 @@
         <v>5</v>
       </c>
       <c r="E38" t="s">
+        <v>126</v>
+      </c>
+      <c r="F38" t="s">
         <v>110</v>
       </c>
-      <c r="G38" t="s">
-        <v>114</v>
-      </c>
       <c r="H38" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="I38" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J38" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K38" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L38" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -2012,22 +2126,25 @@
         <v>8</v>
       </c>
       <c r="E39" t="s">
+        <v>126</v>
+      </c>
+      <c r="F39" t="s">
         <v>112</v>
       </c>
-      <c r="H39" t="s">
-        <v>134</v>
-      </c>
       <c r="I39" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J39" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K39" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L39" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -2041,25 +2158,28 @@
         <v>8</v>
       </c>
       <c r="E40" t="s">
+        <v>126</v>
+      </c>
+      <c r="F40" t="s">
         <v>112</v>
       </c>
-      <c r="G40" t="s">
-        <v>121</v>
-      </c>
       <c r="H40" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="I40" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J40" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K40" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L40" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>23</v>
       </c>
@@ -2073,25 +2193,28 @@
         <v>6</v>
       </c>
       <c r="E41" t="s">
+        <v>126</v>
+      </c>
+      <c r="F41" t="s">
         <v>111</v>
       </c>
-      <c r="G41" t="s">
-        <v>121</v>
-      </c>
       <c r="H41" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="I41" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J41" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K41" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -2105,22 +2228,25 @@
         <v>6</v>
       </c>
       <c r="E42" t="s">
+        <v>126</v>
+      </c>
+      <c r="F42" t="s">
         <v>111</v>
       </c>
-      <c r="H42" t="s">
-        <v>134</v>
-      </c>
       <c r="I42" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J42" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K42" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -2134,22 +2260,25 @@
         <v>7</v>
       </c>
       <c r="E43" t="s">
+        <v>126</v>
+      </c>
+      <c r="F43" t="s">
         <v>108</v>
       </c>
-      <c r="H43" t="s">
-        <v>134</v>
-      </c>
       <c r="I43" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J43" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K43" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -2162,26 +2291,29 @@
       <c r="D44" t="s">
         <v>106</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
         <v>110</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>108</v>
       </c>
-      <c r="H44" t="s">
-        <v>134</v>
-      </c>
       <c r="I44" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J44" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K44" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2194,26 +2326,29 @@
       <c r="D45" t="s">
         <v>106</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45">
+        <v>9</v>
+      </c>
+      <c r="F45" t="s">
         <v>111</v>
       </c>
-      <c r="F45" t="s">
-        <v>118</v>
-      </c>
-      <c r="H45" t="s">
-        <v>134</v>
+      <c r="G45" t="s">
+        <v>117</v>
       </c>
       <c r="I45" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J45" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K45" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -2226,26 +2361,29 @@
       <c r="D46" t="s">
         <v>106</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46">
+        <v>8</v>
+      </c>
+      <c r="F46" t="s">
         <v>110</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>112</v>
       </c>
-      <c r="H46" t="s">
-        <v>134</v>
-      </c>
       <c r="I46" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J46" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K46" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L46" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>68</v>
       </c>
@@ -2258,29 +2396,32 @@
       <c r="D47" t="s">
         <v>106</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47">
+        <v>8</v>
+      </c>
+      <c r="F47" t="s">
+        <v>121</v>
+      </c>
+      <c r="G47" t="s">
         <v>122</v>
       </c>
-      <c r="F47" t="s">
+      <c r="H47" t="s">
         <v>123</v>
       </c>
-      <c r="G47" t="s">
-        <v>124</v>
-      </c>
-      <c r="H47" t="s">
-        <v>134</v>
-      </c>
       <c r="I47" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J47" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K47" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L47" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>20</v>
       </c>
@@ -2293,26 +2434,29 @@
       <c r="D48" t="s">
         <v>106</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48">
+        <v>8</v>
+      </c>
+      <c r="F48" t="s">
         <v>111</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>112</v>
       </c>
-      <c r="H48" t="s">
-        <v>134</v>
-      </c>
       <c r="I48" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J48" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K48" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L48" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -2325,29 +2469,32 @@
       <c r="D49" t="s">
         <v>106</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49">
+        <v>8</v>
+      </c>
+      <c r="F49" t="s">
         <v>111</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>112</v>
       </c>
-      <c r="G49" t="s">
-        <v>119</v>
-      </c>
       <c r="H49" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="I49" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J49" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K49" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L49" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2360,26 +2507,29 @@
       <c r="D50" t="s">
         <v>106</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50">
+        <v>8</v>
+      </c>
+      <c r="F50" t="s">
         <v>110</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>112</v>
       </c>
-      <c r="H50" t="s">
-        <v>134</v>
-      </c>
       <c r="I50" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J50" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K50" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L50" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>87</v>
       </c>
@@ -2392,26 +2542,29 @@
       <c r="D51" t="s">
         <v>106</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51">
+        <v>9</v>
+      </c>
+      <c r="F51" t="s">
         <v>111</v>
       </c>
-      <c r="F51" t="s">
-        <v>118</v>
-      </c>
-      <c r="H51" t="s">
-        <v>134</v>
+      <c r="G51" t="s">
+        <v>117</v>
       </c>
       <c r="I51" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J51" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K51" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L51" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>90</v>
       </c>
@@ -2424,29 +2577,32 @@
       <c r="D52" t="s">
         <v>106</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52">
+        <v>8</v>
+      </c>
+      <c r="F52" t="s">
         <v>110</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>112</v>
       </c>
-      <c r="G52" t="s">
-        <v>125</v>
-      </c>
       <c r="H52" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="I52" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J52" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K52" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L52" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -2459,26 +2615,29 @@
       <c r="D53" t="s">
         <v>106</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53">
+        <v>8</v>
+      </c>
+      <c r="F53" t="s">
         <v>110</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>112</v>
       </c>
-      <c r="H53" t="s">
-        <v>134</v>
-      </c>
       <c r="I53" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J53" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K53" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L53" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -2491,26 +2650,29 @@
       <c r="D54" t="s">
         <v>106</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54">
+        <v>7</v>
+      </c>
+      <c r="F54" t="s">
         <v>107</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>108</v>
       </c>
-      <c r="H54" t="s">
-        <v>134</v>
-      </c>
       <c r="I54" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J54" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K54" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L54" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -2523,26 +2685,29 @@
       <c r="D55" t="s">
         <v>106</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55">
+        <v>8</v>
+      </c>
+      <c r="F55" t="s">
         <v>111</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>112</v>
       </c>
-      <c r="H55" t="s">
-        <v>134</v>
-      </c>
       <c r="I55" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J55" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K55" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L55" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -2555,26 +2720,29 @@
       <c r="D56" t="s">
         <v>106</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56">
+        <v>7</v>
+      </c>
+      <c r="F56" t="s">
         <v>107</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>108</v>
       </c>
-      <c r="H56" t="s">
-        <v>134</v>
-      </c>
       <c r="I56" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J56" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K56" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L56" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>51</v>
       </c>
@@ -2587,79 +2755,82 @@
       <c r="D57" t="s">
         <v>106</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57">
+        <v>8</v>
+      </c>
+      <c r="F57" t="s">
         <v>111</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>112</v>
       </c>
-      <c r="H57" t="s">
-        <v>134</v>
-      </c>
       <c r="I57" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J57" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K57" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L57" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>77</v>
       </c>
       <c r="B58" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>46</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>30</v>
       </c>
       <c r="B60" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>54</v>
       </c>
       <c r="B61" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>76</v>
       </c>
       <c r="B62" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2667,7 +2838,7 @@
         <v>81</v>
       </c>
       <c r="B65" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2675,7 +2846,7 @@
         <v>31</v>
       </c>
       <c r="B66" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2683,7 +2854,7 @@
         <v>79</v>
       </c>
       <c r="B67" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2691,7 +2862,7 @@
         <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2699,7 +2870,7 @@
         <v>80</v>
       </c>
       <c r="B69" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2707,7 +2878,7 @@
         <v>101</v>
       </c>
       <c r="B70" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2715,7 +2886,7 @@
         <v>56</v>
       </c>
       <c r="B71" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2723,7 +2894,7 @@
         <v>102</v>
       </c>
       <c r="B72" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2731,7 +2902,7 @@
         <v>103</v>
       </c>
       <c r="B73" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2739,7 +2910,7 @@
         <v>78</v>
       </c>
       <c r="B74" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2747,7 +2918,7 @@
         <v>105</v>
       </c>
       <c r="B75" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2755,7 +2926,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2763,7 +2934,7 @@
         <v>33</v>
       </c>
       <c r="B77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2771,7 +2942,7 @@
         <v>53</v>
       </c>
       <c r="B78" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2779,7 +2950,7 @@
         <v>89</v>
       </c>
       <c r="B79" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2787,7 +2958,7 @@
         <v>43</v>
       </c>
       <c r="B80" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -2795,7 +2966,7 @@
         <v>28</v>
       </c>
       <c r="B81" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2803,7 +2974,7 @@
         <v>100</v>
       </c>
       <c r="B82" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -2811,7 +2982,7 @@
         <v>29</v>
       </c>
       <c r="B83" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -2819,7 +2990,7 @@
         <v>98</v>
       </c>
       <c r="B84" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2827,7 +2998,7 @@
         <v>74</v>
       </c>
       <c r="B85" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -2835,7 +3006,7 @@
         <v>99</v>
       </c>
       <c r="B86" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -2843,7 +3014,7 @@
         <v>55</v>
       </c>
       <c r="B87" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2939,7 +3110,7 @@
         <v>27</v>
       </c>
       <c r="B99" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2947,7 +3118,7 @@
         <v>58</v>
       </c>
       <c r="B100" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2955,7 +3126,7 @@
         <v>62</v>
       </c>
       <c r="B101" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pulling out brood-specific temperature records + OUNHM name matching
</commit_message>
<xml_diff>
--- a/data/butterfly brood table.xlsx
+++ b/data/butterfly brood table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Butterfly_Project_MBiol\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD9B26C-B06B-4C3B-9231-000967B9BFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160FDED0-889D-4C5D-933E-83441B96CEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{56B928B0-32FD-6245-95ED-D0D0B3954490}"/>
   </bookViews>
@@ -434,12 +434,6 @@
     <t>FirstMonthOf2ndBrood</t>
   </si>
   <si>
-    <t>Brood1_TempDEVELOP </t>
-  </si>
-  <si>
-    <t>Brood2_TempDEVELOP </t>
-  </si>
-  <si>
     <t>Brood1_TempLAY</t>
   </si>
   <si>
@@ -447,6 +441,12 @@
   </si>
   <si>
     <t>NOTES</t>
+  </si>
+  <si>
+    <t>Brood1_TempDEVELOP</t>
+  </si>
+  <si>
+    <t>Brood2_TempDEVELOP</t>
   </si>
 </sst>
 </file>
@@ -527,9 +527,9 @@
     <tableColumn id="5" xr3:uid="{4CA5762C-2EE9-3A42-BD8F-D88788D343F9}" name="Brood 1 dev period"/>
     <tableColumn id="6" xr3:uid="{ED2FC863-549D-CA48-A9C7-55855A1A2F7F}" name="Brood 2 dev period"/>
     <tableColumn id="7" xr3:uid="{6CD8955B-6E7C-564F-B9AF-96E2F29B1E81}" name="NOTES"/>
-    <tableColumn id="8" xr3:uid="{2E6D0983-E3E0-4E2B-8244-A8CDF3940F5E}" name="Brood1_TempDEVELOP "/>
+    <tableColumn id="8" xr3:uid="{2E6D0983-E3E0-4E2B-8244-A8CDF3940F5E}" name="Brood1_TempDEVELOP"/>
     <tableColumn id="9" xr3:uid="{E403E03C-B72B-46C6-B674-8937E304FDB6}" name="Brood1_TempLAY"/>
-    <tableColumn id="10" xr3:uid="{BCBBC58F-E92E-400D-8FFB-43A1E00093CC}" name="Brood2_TempDEVELOP "/>
+    <tableColumn id="10" xr3:uid="{BCBBC58F-E92E-400D-8FFB-43A1E00093CC}" name="Brood2_TempDEVELOP"/>
     <tableColumn id="11" xr3:uid="{49621CBD-7AC2-4720-9EC5-C0CAFFE844A8}" name="Brood2_TempLAY"/>
     <tableColumn id="12" xr3:uid="{2E8ED91B-5795-40A3-9FC4-47B4FFAA76AB}" name="Column2"/>
   </tableColumns>
@@ -857,7 +857,7 @@
   <dimension ref="A1:M101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -895,19 +895,19 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1" t="s">
         <v>136</v>
       </c>
-      <c r="I1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J1" t="s">
-        <v>134</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>133</v>
-      </c>
-      <c r="L1" t="s">
-        <v>135</v>
       </c>
       <c r="M1" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
Setting brood switch months, moving old code to old/
</commit_message>
<xml_diff>
--- a/data/butterfly brood table.xlsx
+++ b/data/butterfly brood table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Butterfly_Project_MBiol\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A95EE1-794A-450F-8FE8-F96086EDECF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67499650-DCA4-49B4-B108-FC58B1CCF194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{56B928B0-32FD-6245-95ED-D0D0B3954490}"/>
+    <workbookView xWindow="-28920" yWindow="5460" windowWidth="29040" windowHeight="15840" xr2:uid="{56B928B0-32FD-6245-95ED-D0D0B3954490}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -929,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A24936-E824-B74E-933F-86465AE8095B}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -941,7 +941,7 @@
     <col min="5" max="5" width="20.25" customWidth="1"/>
     <col min="6" max="6" width="19.125" customWidth="1"/>
     <col min="7" max="7" width="18.375" customWidth="1"/>
-    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="8" max="9" width="15.5" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
     <col min="11" max="11" width="17.125" customWidth="1"/>
   </cols>
@@ -2136,7 +2136,7 @@
         <v>159</v>
       </c>
       <c r="K43">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2200,7 +2200,7 @@
         <v>159</v>
       </c>
       <c r="K45">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -2232,7 +2232,7 @@
         <v>159</v>
       </c>
       <c r="K46">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -2296,7 +2296,7 @@
         <v>159</v>
       </c>
       <c r="K48">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -2331,7 +2331,7 @@
         <v>159</v>
       </c>
       <c r="K49">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -2366,7 +2366,7 @@
         <v>159</v>
       </c>
       <c r="K50">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
         <v>159</v>
       </c>
       <c r="K51">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -2491,7 +2491,7 @@
         <v>159</v>
       </c>
       <c r="K54">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Round off temps and lat longs, tidying names
</commit_message>
<xml_diff>
--- a/data/butterfly brood table.xlsx
+++ b/data/butterfly brood table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Butterfly_Project_MBiol\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67499650-DCA4-49B4-B108-FC58B1CCF194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1DA6A5-EBC1-4B14-B5B6-6EBD7BC59BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5460" windowWidth="29040" windowHeight="15840" xr2:uid="{56B928B0-32FD-6245-95ED-D0D0B3954490}"/>
   </bookViews>
@@ -929,7 +929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A24936-E824-B74E-933F-86465AE8095B}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>

</xml_diff>